<commit_message>
Including a database of cars with marginal elmix
</commit_message>
<xml_diff>
--- a/data/inventory/lci-German-elmix-2018.xlsx
+++ b/data/inventory/lci-German-elmix-2018.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="74">
   <si>
     <t>Database</t>
   </si>
@@ -228,9 +228,6 @@
   </si>
   <si>
     <t>treatment of coal gas, in power plant</t>
-  </si>
-  <si>
-    <t>market for electricity, high voltage</t>
   </si>
   <si>
     <t>electricity production, photovoltaic, 3kWp slanted-roof installation, multi-Si, panel, mounted</t>
@@ -642,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,7 +1371,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="B48" s="5">
         <v>1.9262732000000001E-2</v>
@@ -1737,7 +1734,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B81" s="5">
         <v>4.9421396999999999E-2</v>
@@ -1754,7 +1751,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B82" s="5">
         <v>3.9681362999999997E-2</v>
@@ -1771,7 +1768,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B83" s="5">
         <v>3.0823603000000002E-2</v>
@@ -1788,7 +1785,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B84" s="5">
         <v>0.88007363699999996</v>
@@ -1805,7 +1802,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B85" s="5">
         <v>1.7314360000000001E-2</v>
@@ -1822,7 +1819,7 @@
     </row>
     <row r="86" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A86" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B86" s="6">
         <v>8.7404999999999994E-8</v>
@@ -1859,7 +1856,7 @@
         <v>3</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -1867,7 +1864,7 @@
         <v>4</v>
       </c>
       <c r="B90" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -1883,7 +1880,7 @@
         <v>6</v>
       </c>
       <c r="B92" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>